<commit_message>
[Modify]: Fix bugs (#134)
</commit_message>
<xml_diff>
--- a/src/assets/ExcelExampleEnergy/ImportFile.xlsx
+++ b/src/assets/ExcelExampleEnergy/ImportFile.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VNPTBPC\tuhla.bpc\Coding\SCT\industrial-and-commercial-facilities\src\assets\ExcelExampleEnergy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5AA9CC-493F-4969-AEED-02BBACA6A20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="876" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="876" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Điện mặt trời" sheetId="1" r:id="rId1"/>
@@ -36,7 +35,7 @@
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="459">
   <si>
     <t>MẪU NHẬP LIỆU ĐIỆN MẶT TRỜI</t>
   </si>
@@ -1450,7 +1449,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1527,7 +1526,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1559,49 +1558,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1638,19 +1600,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2144,29 +2100,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2189,7 +2145,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2232,7 +2188,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -2258,7 +2214,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -2271,7 +2227,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2284,7 +2240,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -2297,7 +2253,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -2310,7 +2266,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -2323,7 +2279,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -2336,7 +2292,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -2349,7 +2305,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2362,7 +2318,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2375,7 +2331,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2388,7 +2344,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2401,7 +2357,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -2414,7 +2370,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -2427,7 +2383,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2440,7 +2396,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2453,7 +2409,7 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -2475,7 +2431,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Quận, huyện'!$A$2:$A$12</xm:f>
           </x14:formula1>
@@ -2488,29 +2444,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>433</v>
       </c>
@@ -2525,7 +2481,7 @@
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2560,7 +2516,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -2597,7 +2553,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -2610,7 +2566,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2623,7 +2579,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -2636,7 +2592,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -2649,7 +2605,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -2662,7 +2618,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -2675,7 +2631,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -2688,7 +2644,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2701,7 +2657,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2714,7 +2670,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2727,7 +2683,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2740,7 +2696,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -2753,7 +2709,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -2766,7 +2722,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2779,7 +2735,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2792,7 +2748,7 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -2810,7 +2766,7 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3">
       <formula1>"Giai đoạn 2021-2030, Giai đoạn 2031-2050"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2818,7 +2774,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Loại trạm'!$A2:$A4</xm:f>
           </x14:formula1>
@@ -2831,30 +2787,30 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
     <col min="9" max="9" width="20" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>433</v>
       </c>
@@ -2870,7 +2826,7 @@
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2908,7 +2864,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -2949,7 +2905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -2963,7 +2919,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2977,7 +2933,7 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -2991,7 +2947,7 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -3005,7 +2961,7 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -3019,7 +2975,7 @@
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -3033,7 +2989,7 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -3047,7 +3003,7 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -3061,7 +3017,7 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -3075,7 +3031,7 @@
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -3089,7 +3045,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -3103,7 +3059,7 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -3117,7 +3073,7 @@
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -3131,7 +3087,7 @@
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -3145,7 +3101,7 @@
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -3159,7 +3115,7 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -3178,7 +3134,7 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3">
       <formula1>"Giai đoạn 2021-2030, Giai đoạn 2031-2050"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3186,13 +3142,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Loại công trình'!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>G3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0A00-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Quận, huyện'!$A$2:$A$12</xm:f>
           </x14:formula1>
@@ -3205,79 +3161,87 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0666A8-E351-438A-B68C-7CBEF3C05C61}">
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>458</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="12" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -3289,8 +3253,10 @@
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -3302,8 +3268,10 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -3315,8 +3283,10 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -3328,8 +3298,10 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -3341,8 +3313,10 @@
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -3354,8 +3328,10 @@
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -3367,8 +3343,10 @@
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -3380,8 +3358,10 @@
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -3393,8 +3373,10 @@
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -3406,8 +3388,10 @@
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -3419,10 +3403,12 @@
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3430,19 +3416,19 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>387</v>
       </c>
@@ -3450,7 +3436,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>438</v>
       </c>
@@ -3458,7 +3444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>439</v>
       </c>
@@ -3466,7 +3452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>440</v>
       </c>
@@ -3474,7 +3460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>441</v>
       </c>
@@ -3488,20 +3474,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>387</v>
       </c>
@@ -3509,7 +3495,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>432</v>
       </c>
@@ -3517,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>445</v>
       </c>
@@ -3531,19 +3517,19 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>387</v>
       </c>
@@ -3551,7 +3537,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>401</v>
       </c>
@@ -3559,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>402</v>
       </c>
@@ -3567,7 +3553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>403</v>
       </c>
@@ -3582,20 +3568,20 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="1.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>386</v>
       </c>
@@ -3606,7 +3592,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -3617,7 +3603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -3628,7 +3614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -3639,7 +3625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -3657,24 +3643,24 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>273</v>
       </c>
@@ -3694,7 +3680,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>274</v>
       </c>
@@ -3715,7 +3701,7 @@
         <v>Phường Tân Phú, Thành phố Đồng Xoài</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>384</v>
       </c>
@@ -3736,7 +3722,7 @@
         <v>Phường Tân Đồng, Thành phố Đồng Xoài</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>383</v>
       </c>
@@ -3757,7 +3743,7 @@
         <v>Phường Tân Bình, Thành phố Đồng Xoài</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>382</v>
       </c>
@@ -3778,7 +3764,7 @@
         <v>Phường Tân Xuân, Thành phố Đồng Xoài</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>381</v>
       </c>
@@ -3799,7 +3785,7 @@
         <v>Phường Tân Thiện, Thành phố Đồng Xoài</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>380</v>
       </c>
@@ -3820,7 +3806,7 @@
         <v>Xã Tân Thành, Thành phố Đồng Xoài</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>379</v>
       </c>
@@ -3841,7 +3827,7 @@
         <v>Phường Tiến Thành, Thành phố Đồng Xoài</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>378</v>
       </c>
@@ -3862,7 +3848,7 @@
         <v>Xã Tiến Hưng, Thành phố Đồng Xoài</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>377</v>
       </c>
@@ -3883,7 +3869,7 @@
         <v>Phường Thác Mơ, Thị xã Phước Long</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>376</v>
       </c>
@@ -3904,7 +3890,7 @@
         <v>Phường Long Thủy, Thị xã Phước Long</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>375</v>
       </c>
@@ -3925,7 +3911,7 @@
         <v>Phường Phước Bình, Thị xã Phước Long</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>374</v>
       </c>
@@ -3946,7 +3932,7 @@
         <v>Phường Long Phước, Thị xã Phước Long</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>373</v>
       </c>
@@ -3967,7 +3953,7 @@
         <v>Xã Bù Gia Mập, Huyện Bù Gia Mập</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>372</v>
       </c>
@@ -3988,7 +3974,7 @@
         <v>Xã Đak Ơ, Huyện Bù Gia Mập</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>371</v>
       </c>
@@ -4009,7 +3995,7 @@
         <v>Xã Đức Hạnh, Huyện Bù Gia Mập</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>370</v>
       </c>
@@ -4030,7 +4016,7 @@
         <v>Xã Phú Văn, Huyện Bù Gia Mập</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>369</v>
       </c>
@@ -4051,7 +4037,7 @@
         <v>Xã Đa Kia, Huyện Bù Gia Mập</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>368</v>
       </c>
@@ -4072,7 +4058,7 @@
         <v>Xã Phước Minh, Huyện Bù Gia Mập</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>367</v>
       </c>
@@ -4093,7 +4079,7 @@
         <v>Xã Bình Thắng, Huyện Bù Gia Mập</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>366</v>
       </c>
@@ -4114,7 +4100,7 @@
         <v>Phường Sơn Giang, Thị xã Phước Long</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>365</v>
       </c>
@@ -4135,7 +4121,7 @@
         <v>Xã Long Bình, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>364</v>
       </c>
@@ -4156,7 +4142,7 @@
         <v>Xã Bình Tân, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>363</v>
       </c>
@@ -4177,7 +4163,7 @@
         <v>Xã Bình Sơn, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>362</v>
       </c>
@@ -4198,7 +4184,7 @@
         <v>Xã Long Giang, Thị xã Phước Long</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>361</v>
       </c>
@@ -4219,7 +4205,7 @@
         <v>Xã Long Hưng, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>360</v>
       </c>
@@ -4240,7 +4226,7 @@
         <v>Xã Phước Tín, Thị xã Phước Long</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>359</v>
       </c>
@@ -4261,7 +4247,7 @@
         <v>Xã Phước Tân, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>358</v>
       </c>
@@ -4282,7 +4268,7 @@
         <v>Xã Bù Nho, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>357</v>
       </c>
@@ -4303,7 +4289,7 @@
         <v>Xã Long Hà, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>356</v>
       </c>
@@ -4324,7 +4310,7 @@
         <v>Xã Long Tân, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>355</v>
       </c>
@@ -4345,7 +4331,7 @@
         <v>Xã Phú Trung, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>354</v>
       </c>
@@ -4366,7 +4352,7 @@
         <v>Xã Phú Riềng, Huyện Phú Riềng</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>353</v>
       </c>
@@ -4387,7 +4373,7 @@
         <v>Xã Phú Nghĩa, Huyện Bù Gia Mập</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>352</v>
       </c>
@@ -4408,7 +4394,7 @@
         <v>Thị trấn Lộc Ninh, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>351</v>
       </c>
@@ -4429,7 +4415,7 @@
         <v>Xã Lộc Hòa, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>350</v>
       </c>
@@ -4450,7 +4436,7 @@
         <v>Xã Lộc An, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>349</v>
       </c>
@@ -4471,7 +4457,7 @@
         <v>Xã Lộc Tấn, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>348</v>
       </c>
@@ -4492,7 +4478,7 @@
         <v>Xã Lộc Thạnh, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>347</v>
       </c>
@@ -4513,7 +4499,7 @@
         <v>Xã Lộc Hiệp, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>346</v>
       </c>
@@ -4534,7 +4520,7 @@
         <v>Xã Lộc Thiện, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>345</v>
       </c>
@@ -4555,7 +4541,7 @@
         <v>Xã Lộc Thuận, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>344</v>
       </c>
@@ -4576,7 +4562,7 @@
         <v>Xã Lộc Quang, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>343</v>
       </c>
@@ -4597,7 +4583,7 @@
         <v>Xã Lộc Phú, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
         <v>342</v>
       </c>
@@ -4618,7 +4604,7 @@
         <v>Xã Lộc Thành, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>341</v>
       </c>
@@ -4639,7 +4625,7 @@
         <v>Xã Lộc Thái, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>340</v>
       </c>
@@ -4660,7 +4646,7 @@
         <v>Xã Lộc Điền, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>339</v>
       </c>
@@ -4681,7 +4667,7 @@
         <v>Xã Lộc Hưng, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>338</v>
       </c>
@@ -4702,7 +4688,7 @@
         <v>Xã Lộc Thịnh, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>337</v>
       </c>
@@ -4723,7 +4709,7 @@
         <v>Xã Lộc Khánh, Huyện Lộc Ninh</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>336</v>
       </c>
@@ -4744,7 +4730,7 @@
         <v>Thị trấn Thanh Bình, Huyện Bù Đốp</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>335</v>
       </c>
@@ -4765,7 +4751,7 @@
         <v>Xã Hưng Phước, Huyện Bù Đốp</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>334</v>
       </c>
@@ -4786,7 +4772,7 @@
         <v>Xã Phước Thiện, Huyện Bù Đốp</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>333</v>
       </c>
@@ -4807,7 +4793,7 @@
         <v>Xã Thiện Hưng, Huyện Bù Đốp</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>332</v>
       </c>
@@ -4828,7 +4814,7 @@
         <v>Xã Thanh Hòa, Huyện Bù Đốp</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>331</v>
       </c>
@@ -4849,7 +4835,7 @@
         <v>Xã Tân Thành, Huyện Bù Đốp</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
         <v>330</v>
       </c>
@@ -4870,7 +4856,7 @@
         <v>Phường Hưng Chiến, Thị xã Bình Long</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
         <v>329</v>
       </c>
@@ -4891,7 +4877,7 @@
         <v>Xã Tân Tiến, Huyện Bù Đốp</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>328</v>
       </c>
@@ -4912,7 +4898,7 @@
         <v>Phường An Lộc, Thị xã Bình Long</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
         <v>327</v>
       </c>
@@ -4933,7 +4919,7 @@
         <v>Phường Phú Thịnh, Thị xã Bình Long</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
         <v>326</v>
       </c>
@@ -4954,7 +4940,7 @@
         <v>Phường Phú Đức, Thị xã Bình Long</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
         <v>325</v>
       </c>
@@ -4975,7 +4961,7 @@
         <v>Xã Thanh An, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
         <v>324</v>
       </c>
@@ -4996,7 +4982,7 @@
         <v>Xã An Khương, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>323</v>
       </c>
@@ -5017,7 +5003,7 @@
         <v>Xã Thanh Lương, Thị xã Bình Long</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
         <v>322</v>
       </c>
@@ -5038,7 +5024,7 @@
         <v>Xã Thanh Phú, Thị xã Bình Long</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>321</v>
       </c>
@@ -5059,7 +5045,7 @@
         <v>Xã An Phú, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
         <v>320</v>
       </c>
@@ -5080,7 +5066,7 @@
         <v>Xã Tân Lợi, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>319</v>
       </c>
@@ -5101,7 +5087,7 @@
         <v>Xã Tân Hưng, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
         <v>318</v>
       </c>
@@ -5122,7 +5108,7 @@
         <v>Xã Minh Đức, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
         <v>317</v>
       </c>
@@ -5143,7 +5129,7 @@
         <v>Xã Minh Tâm, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
         <v>316</v>
       </c>
@@ -5164,7 +5150,7 @@
         <v>Xã Phước An, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
         <v>315</v>
       </c>
@@ -5185,7 +5171,7 @@
         <v>Xã Thanh Bình, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
         <v>314</v>
       </c>
@@ -5206,7 +5192,7 @@
         <v>Thị trấn Tân Khai, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
         <v>313</v>
       </c>
@@ -5227,7 +5213,7 @@
         <v>Xã Đồng Nơ, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
         <v>312</v>
       </c>
@@ -5248,7 +5234,7 @@
         <v>Xã Tân Hiệp, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>311</v>
       </c>
@@ -5269,7 +5255,7 @@
         <v>Thị trấn Tân Phú, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
         <v>310</v>
       </c>
@@ -5290,7 +5276,7 @@
         <v>Xã Thuận Lợi, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
         <v>309</v>
       </c>
@@ -5311,7 +5297,7 @@
         <v>Xã Đồng Tâm, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
         <v>308</v>
       </c>
@@ -5332,7 +5318,7 @@
         <v>Xã Tân Phước, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="12" t="s">
         <v>307</v>
       </c>
@@ -5353,7 +5339,7 @@
         <v>Xã Tân Hưng, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
         <v>306</v>
       </c>
@@ -5374,7 +5360,7 @@
         <v>Xã Tân Lợi, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
         <v>305</v>
       </c>
@@ -5395,7 +5381,7 @@
         <v>Xã Tân Lập, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
         <v>304</v>
       </c>
@@ -5416,7 +5402,7 @@
         <v>Xã Tân Hòa, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="12" t="s">
         <v>303</v>
       </c>
@@ -5437,7 +5423,7 @@
         <v>Xã Thuận Phú, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
         <v>302</v>
       </c>
@@ -5458,7 +5444,7 @@
         <v>Xã Đồng Tiến, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
         <v>301</v>
       </c>
@@ -5479,7 +5465,7 @@
         <v>Xã Tân Tiến, Huyện Đồng Phú</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
         <v>300</v>
       </c>
@@ -5500,7 +5486,7 @@
         <v>Thị trấn Đức Phong, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
         <v>299</v>
       </c>
@@ -5521,7 +5507,7 @@
         <v>Xã Đường 10, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
         <v>298</v>
       </c>
@@ -5542,7 +5528,7 @@
         <v>Xã Đak Nhau, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
         <v>297</v>
       </c>
@@ -5563,7 +5549,7 @@
         <v>Xã Phú Sơn, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="12" t="s">
         <v>296</v>
       </c>
@@ -5584,7 +5570,7 @@
         <v>Xã Thọ Sơn, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
         <v>295</v>
       </c>
@@ -5605,7 +5591,7 @@
         <v>Xã Bình Minh, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
         <v>294</v>
       </c>
@@ -5626,7 +5612,7 @@
         <v>Xã Bom Bo, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
         <v>293</v>
       </c>
@@ -5647,7 +5633,7 @@
         <v>Xã Minh Hưng, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
         <v>292</v>
       </c>
@@ -5668,7 +5654,7 @@
         <v>Xã Đoàn Kết, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
         <v>291</v>
       </c>
@@ -5689,7 +5675,7 @@
         <v>Xã Đồng Nai, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
         <v>290</v>
       </c>
@@ -5710,7 +5696,7 @@
         <v>Xã Đức Liễu, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
         <v>289</v>
       </c>
@@ -5731,7 +5717,7 @@
         <v>Xã Thống Nhất, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
         <v>288</v>
       </c>
@@ -5752,7 +5738,7 @@
         <v>Xã Nghĩa Trung, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
         <v>287</v>
       </c>
@@ -5773,7 +5759,7 @@
         <v>Xã Nghĩa Bình, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
         <v>286</v>
       </c>
@@ -5794,7 +5780,7 @@
         <v>Xã Đăng Hà, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
         <v>285</v>
       </c>
@@ -5815,7 +5801,7 @@
         <v>Xã Phước Sơn, Huyện Bù Đăng</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
         <v>284</v>
       </c>
@@ -5836,7 +5822,7 @@
         <v>Thị trấn Chơn Thành, Huyện Chơn Thành</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
         <v>283</v>
       </c>
@@ -5857,7 +5843,7 @@
         <v>Xã Thành Tâm, Huyện Chơn Thành</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
         <v>282</v>
       </c>
@@ -5878,7 +5864,7 @@
         <v>Xã Minh Lập, Huyện Chơn Thành</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
         <v>281</v>
       </c>
@@ -5899,7 +5885,7 @@
         <v>Xã Tân Quan, Huyện Hớn Quản</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
         <v>280</v>
       </c>
@@ -5920,7 +5906,7 @@
         <v>Xã Quang Minh, Huyện Chơn Thành</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="12" t="s">
         <v>279</v>
       </c>
@@ -5941,7 +5927,7 @@
         <v>Xã Minh Hưng, Huyện Chơn Thành</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="12" t="s">
         <v>278</v>
       </c>
@@ -5962,7 +5948,7 @@
         <v>Xã Minh Long, Huyện Chơn Thành</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="12" t="s">
         <v>277</v>
       </c>
@@ -5983,7 +5969,7 @@
         <v>Xã Minh Thành, Huyện Chơn Thành</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
         <v>276</v>
       </c>
@@ -6004,7 +5990,7 @@
         <v>Xã Nha Bích, Huyện Chơn Thành</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
         <v>275</v>
       </c>
@@ -6031,20 +6017,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -6052,7 +6038,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -6060,7 +6046,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -6068,7 +6054,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -6076,7 +6062,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -6084,7 +6070,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -6092,7 +6078,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
@@ -6100,7 +6086,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -6108,7 +6094,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -6116,7 +6102,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -6124,7 +6110,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
@@ -6132,7 +6118,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -6146,37 +6132,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.109375" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>27</v>
       </c>
@@ -6206,7 +6192,7 @@
       <c r="Y1" s="15"/>
       <c r="Z1" s="15"/>
     </row>
-    <row r="2" spans="1:26" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -6286,7 +6272,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -6368,7 +6354,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -6396,7 +6382,7 @@
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -6424,7 +6410,7 @@
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -6452,7 +6438,7 @@
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -6480,7 +6466,7 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -6508,7 +6494,7 @@
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -6536,7 +6522,7 @@
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -6564,7 +6550,7 @@
       <c r="Y10" s="8"/>
       <c r="Z10" s="8"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -6592,7 +6578,7 @@
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -6620,7 +6606,7 @@
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -6648,7 +6634,7 @@
       <c r="Y13" s="8"/>
       <c r="Z13" s="8"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -6676,7 +6662,7 @@
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -6704,7 +6690,7 @@
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -6732,7 +6718,7 @@
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -6760,7 +6746,7 @@
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -6788,7 +6774,7 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -6825,7 +6811,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Xã, phường'!F$2:F$112</xm:f>
           </x14:formula1>
@@ -6838,29 +6824,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="15" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>385</v>
       </c>
@@ -6875,7 +6861,7 @@
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -6910,7 +6896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -6946,7 +6932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -6959,7 +6945,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -6972,7 +6958,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -6985,7 +6971,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -6998,7 +6984,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -7011,7 +6997,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -7024,7 +7010,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -7037,7 +7023,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -7050,7 +7036,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -7063,7 +7049,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -7076,7 +7062,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -7089,7 +7075,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -7102,7 +7088,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -7115,7 +7101,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -7128,7 +7114,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -7141,7 +7127,7 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -7162,7 +7148,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Quận, huyện'!$A$2:$A$12</xm:f>
           </x14:formula1>
@@ -7175,29 +7161,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>416</v>
       </c>
@@ -7212,7 +7198,7 @@
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -7247,7 +7233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -7283,7 +7269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -7296,7 +7282,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -7309,7 +7295,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -7322,7 +7308,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -7335,7 +7321,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -7348,7 +7334,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -7361,7 +7347,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -7374,7 +7360,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -7387,7 +7373,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -7400,7 +7386,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -7413,7 +7399,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -7426,7 +7412,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -7439,7 +7425,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -7452,7 +7438,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -7465,7 +7451,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -7478,7 +7464,7 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -7499,7 +7485,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Quận, huyện'!$A$2:$A$12</xm:f>
           </x14:formula1>
@@ -7512,28 +7498,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>417</v>
       </c>
@@ -7547,7 +7533,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -7579,7 +7565,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -7612,7 +7598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -7624,7 +7610,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -7636,7 +7622,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -7648,7 +7634,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -7660,7 +7646,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -7672,7 +7658,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -7684,7 +7670,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -7696,7 +7682,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -7708,7 +7694,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -7720,7 +7706,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -7732,7 +7718,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -7744,7 +7730,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -7756,7 +7742,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -7768,7 +7754,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -7780,7 +7766,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -7792,7 +7778,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -7812,7 +7798,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Loại đường dây'!B$2:B$5</xm:f>
           </x14:formula1>
@@ -7825,27 +7811,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>418</v>
       </c>
@@ -7858,7 +7844,7 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -7887,7 +7873,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -7917,7 +7903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -7928,7 +7914,7 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -7939,7 +7925,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -7950,7 +7936,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -7961,7 +7947,7 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -7972,7 +7958,7 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -7983,7 +7969,7 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -7994,7 +7980,7 @@
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -8005,7 +7991,7 @@
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -8016,7 +8002,7 @@
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -8027,7 +8013,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -8038,7 +8024,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -8049,7 +8035,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -8060,7 +8046,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -8071,7 +8057,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -8082,7 +8068,7 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -8101,7 +8087,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Loại trạm'!$A$2:$A$4</xm:f>
           </x14:formula1>
@@ -8114,26 +8100,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>419</v>
       </c>
@@ -8147,7 +8133,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -8179,7 +8165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -8212,7 +8198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -8224,7 +8210,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -8236,7 +8222,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -8248,7 +8234,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -8260,7 +8246,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -8272,7 +8258,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -8284,7 +8270,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -8296,7 +8282,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -8308,7 +8294,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -8320,7 +8306,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -8332,7 +8318,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -8344,7 +8330,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -8356,7 +8342,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -8368,7 +8354,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -8380,7 +8366,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -8392,7 +8378,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -8412,7 +8398,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'C:\Users\VNPTBPC\Downloads\[Mẫu import (4).xlsx]Quận, huyện'!#REF!</xm:f>
           </x14:formula1>
@@ -8425,27 +8411,27 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
     <col min="4" max="4" width="15" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>443</v>
       </c>
@@ -8458,7 +8444,7 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -8487,7 +8473,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -8517,7 +8503,7 @@
         <v>47760</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -8528,7 +8514,7 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -8539,7 +8525,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -8550,7 +8536,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -8561,7 +8547,7 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -8572,7 +8558,7 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -8583,7 +8569,7 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -8594,7 +8580,7 @@
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -8605,7 +8591,7 @@
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -8616,7 +8602,7 @@
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -8627,7 +8613,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -8638,7 +8624,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -8649,7 +8635,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -8660,7 +8646,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -8671,7 +8657,7 @@
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -8682,7 +8668,7 @@
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -8702,7 +8688,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Quận, huyện'!$A$2:$A$12</xm:f>
           </x14:formula1>
@@ -8715,28 +8701,28 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G2" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="28.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>424</v>
       </c>
@@ -8750,7 +8736,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -8782,7 +8768,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -8816,7 +8802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -8828,7 +8814,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -8840,7 +8826,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -8852,7 +8838,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -8864,7 +8850,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -8876,7 +8862,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -8888,7 +8874,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -8900,7 +8886,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -8912,7 +8898,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -8924,7 +8910,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -8936,7 +8922,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -8948,7 +8934,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -8960,7 +8946,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -8972,7 +8958,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -8984,7 +8970,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -8996,7 +8982,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -9013,7 +8999,7 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3">
       <formula1>"Giai đoạn 2021-2030, Giai đoạn 2031-2050"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9021,7 +9007,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Loại đường dây'!$B$2:$B$5</xm:f>
           </x14:formula1>

</xml_diff>